<commit_message>
Primer caso de prueba creado, sin errores. Se modificaron varias cosas del codigo con respecto a la versión anterior partiendo con lo aprendido en el curso hasta amoldarlo a lo que yo necesito.
</commit_message>
<xml_diff>
--- a/src/test/resources/datos/DataDriven.xlsx
+++ b/src/test/resources/datos/DataDriven.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose.Valdez\Documents\TrabajoPOM_Valdez\src\test\resources\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Documents\dev\automatizacion\TrabajoPOM_Valdez\src\test\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBB2178-6939-42BF-8FA8-9FF7CD3248C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477F0E2B-CE1F-4192-9C33-2DE20D3BA2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="4470" activeTab="1" xr2:uid="{91E5DE3C-F75B-4810-A43F-47BF2AD7F516}"/>
+    <workbookView xWindow="7335" yWindow="4095" windowWidth="18630" windowHeight="11325" xr2:uid="{91E5DE3C-F75B-4810-A43F-47BF2AD7F516}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="DatosCP" sheetId="2" r:id="rId2"/>
+    <sheet name="DatosCP" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
-  <si>
-    <t>CP001</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>CP002</t>
   </si>
@@ -55,12 +51,6 @@
     <t>CasosDePrueba</t>
   </si>
   <si>
-    <t>dato1CP1</t>
-  </si>
-  <si>
-    <t>CP12</t>
-  </si>
-  <si>
     <t>CP22</t>
   </si>
   <si>
@@ -70,9 +60,6 @@
     <t>CP52</t>
   </si>
   <si>
-    <t>CP13</t>
-  </si>
-  <si>
     <t>CP23</t>
   </si>
   <si>
@@ -91,13 +78,16 @@
     <t>dato4CP1</t>
   </si>
   <si>
-    <t>CP001_retomaFormularioContratacion</t>
-  </si>
-  <si>
-    <t>11082485-8</t>
-  </si>
-  <si>
-    <t>Superaste el número de intentos y por seguridad bloqueamos tu cuenta. Espera 24 hrs e inténtalo nuevamente.</t>
+    <t>qweqweew</t>
+  </si>
+  <si>
+    <t>ee51165</t>
+  </si>
+  <si>
+    <t>CP001_loginInvalidEmail</t>
+  </si>
+  <si>
+    <t>Invalid email address.</t>
   </si>
 </sst>
 </file>
@@ -156,15 +146,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,111 +465,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5872D5CB-4F9B-473F-9D09-72B4B3B4964C}">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F35BA004-4740-4C28-B5A6-AA18427F295D}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -592,90 +474,90 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="7"/>
+    <col min="1" max="1" width="35.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="5">
-        <v>123123123</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>23</v>
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregaron más casos de prueba. Haciendo un total de 4
</commit_message>
<xml_diff>
--- a/src/test/resources/datos/DataDriven.xlsx
+++ b/src/test/resources/datos/DataDriven.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Documents\dev\automatizacion\TrabajoPOM_Valdez\src\test\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477F0E2B-CE1F-4192-9C33-2DE20D3BA2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C53E08-4481-48BA-B8D0-BE1FDF0DB05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7335" yWindow="4095" windowWidth="18630" windowHeight="11325" xr2:uid="{91E5DE3C-F75B-4810-A43F-47BF2AD7F516}"/>
+    <workbookView xWindow="3345" yWindow="1665" windowWidth="18630" windowHeight="11325" xr2:uid="{91E5DE3C-F75B-4810-A43F-47BF2AD7F516}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCP" sheetId="2" r:id="rId1"/>
@@ -25,19 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
-  <si>
-    <t>CP002</t>
-  </si>
-  <si>
-    <t>CP003</t>
-  </si>
-  <si>
-    <t>CP004</t>
-  </si>
-  <si>
-    <t>CP005</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>dato 1</t>
   </si>
@@ -51,33 +39,6 @@
     <t>CasosDePrueba</t>
   </si>
   <si>
-    <t>CP22</t>
-  </si>
-  <si>
-    <t>CP32</t>
-  </si>
-  <si>
-    <t>CP52</t>
-  </si>
-  <si>
-    <t>CP23</t>
-  </si>
-  <si>
-    <t>CP33</t>
-  </si>
-  <si>
-    <t>CP53</t>
-  </si>
-  <si>
-    <t>dato2CP1</t>
-  </si>
-  <si>
-    <t>dato3CP1</t>
-  </si>
-  <si>
-    <t>dato4CP1</t>
-  </si>
-  <si>
     <t>qweqweew</t>
   </si>
   <si>
@@ -88,13 +49,43 @@
   </si>
   <si>
     <t>Invalid email address.</t>
+  </si>
+  <si>
+    <t>fakemail@gmail.com</t>
+  </si>
+  <si>
+    <t>Authentication failed.</t>
+  </si>
+  <si>
+    <t>asdffgr2</t>
+  </si>
+  <si>
+    <t>CP002_loginEmail</t>
+  </si>
+  <si>
+    <t>mailtestautomation001@gmail.com</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Welcome to your account. Here you can manage all of your personal information and orders.</t>
+  </si>
+  <si>
+    <t>CP003_logInSuccessfully</t>
+  </si>
+  <si>
+    <t>CP004_AddProductToWishlist</t>
+  </si>
+  <si>
+    <t>Added to your wishlist.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +97,20 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,17 +148,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -466,102 +475,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F35BA004-4740-4C28-B5A6-AA18427F295D}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="3"/>
+    <col min="2" max="3" width="11.42578125" style="3"/>
+    <col min="4" max="4" width="84.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{362EDAA9-A861-4A3F-986F-5F6A6F8D1447}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{A23BFC85-55C4-431A-83B3-19D5EE0DDE2F}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{BFBA1DE9-6602-432E-B340-3AC476C8558A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agregan los casos que faltaban, para hacer un total de 8. Tambien se sube la carpeta target con todos los casos en passed.
</commit_message>
<xml_diff>
--- a/src/test/resources/datos/DataDriven.xlsx
+++ b/src/test/resources/datos/DataDriven.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Documents\dev\automatizacion\TrabajoPOM_Valdez\src\test\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C53E08-4481-48BA-B8D0-BE1FDF0DB05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5A8174-95E4-4D33-AFC7-741146FC091D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3345" yWindow="1665" windowWidth="18630" windowHeight="11325" xr2:uid="{91E5DE3C-F75B-4810-A43F-47BF2AD7F516}"/>
+    <workbookView xWindow="6900" yWindow="3480" windowWidth="18630" windowHeight="11325" xr2:uid="{91E5DE3C-F75B-4810-A43F-47BF2AD7F516}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCP" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>dato 1</t>
   </si>
@@ -75,10 +75,28 @@
     <t>CP003_logInSuccessfully</t>
   </si>
   <si>
-    <t>CP004_AddProductToWishlist</t>
-  </si>
-  <si>
     <t>Added to your wishlist.</t>
+  </si>
+  <si>
+    <t>CP005_checkThatProductAppearsonWantedList</t>
+  </si>
+  <si>
+    <t>CP006_searchProductNotAddedToWishList</t>
+  </si>
+  <si>
+    <t>CP004_addProductToWishlist</t>
+  </si>
+  <si>
+    <t>Product successfully added to your shopping cart</t>
+  </si>
+  <si>
+    <t>CP007_agregarProductoSinLogin</t>
+  </si>
+  <si>
+    <t>Your shopping cart is empty.</t>
+  </si>
+  <si>
+    <t>CP008_emptyCartMessage</t>
   </si>
 </sst>
 </file>
@@ -152,14 +170,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -475,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F35BA004-4740-4C28-B5A6-AA18427F295D}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +555,7 @@
       <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -547,16 +564,68 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -565,8 +634,12 @@
     <hyperlink ref="B3" r:id="rId1" xr:uid="{362EDAA9-A861-4A3F-986F-5F6A6F8D1447}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{A23BFC85-55C4-431A-83B3-19D5EE0DDE2F}"/>
     <hyperlink ref="B5" r:id="rId3" xr:uid="{BFBA1DE9-6602-432E-B340-3AC476C8558A}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{71CC9A1F-7A87-4FA8-82DC-CE72F5CCBE28}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{06C4176D-1734-4463-9472-45989D32CCF0}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{A04536B0-25A8-4CC5-8001-E6A17FCB7F19}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{A9D2F373-F58C-43AE-A558-C321BAF5DFC5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>